<commit_message>
updated dataset and code
</commit_message>
<xml_diff>
--- a/QA Questions CoyPu.xlsx
+++ b/QA Questions CoyPu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longquan/Documents/Workspace/coypu-KGQA-Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E14867-1AE6-4947-9D97-B76999087599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD223FD5-778C-5046-96A7-853936AACDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>Wie lautet das internationale Kürzel von Saudi-Arabien?</t>
   </si>
   <si>
-    <t>SELECT ?result WHERE {&lt;https://data.coypu.org/country/SAU&gt; coy:hasIso3Code ?result .}</t>
-  </si>
-  <si>
     <t>What are the last three natural disasters with level orange?</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
   </si>
   <si>
     <t>Wie ist das Risiko-Level von Deutschland?</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT ?result WHERE {&lt;https://data.coypu.org/country/DEU&gt; coy:hasRiskLevel ?result .}</t>
   </si>
   <si>
     <t>How many disasters happened in 2021 with level 1 or orange?</t>
@@ -773,6 +767,12 @@
   </si>
   <si>
     <t>ASK { ?subject coy:hasLocation ?country; coy:hasInfrastructureType "port"; rdfs:label "Tokyo" . ?country rdf:type coy:Country; rdfs:label "Japan"@en.}</t>
+  </si>
+  <si>
+    <t>SELECT ?result WHERE {?subject rdf:type coy:Country ; rdfs:label "Saudi Arabia"@en ; coy:hasIsoCode ?result .}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?result WHERE { ?subject rdf:type coy:Country ; rdfs:label "Germany"@en; coy:hasRiskLevel ?result .}</t>
   </si>
 </sst>
 </file>
@@ -1172,8 +1172,8 @@
   </sheetPr>
   <dimension ref="A1:Z937"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1224,7 +1224,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1268,425 +1268,425 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="126" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -4393,432 +4393,432 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B15" s="12"/>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B19" s="12"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B28" s="12"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B34" s="12"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>